<commit_message>
continuity and diffrenciability modified
</commit_message>
<xml_diff>
--- a/12/12ContinuityAndDiffrentiability.xlsx
+++ b/12/12ContinuityAndDiffrentiability.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19635" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">1) </t>
   </si>
@@ -121,38 +121,14 @@
     <t>sin(x+y) = sin(x)cos(y) + cos(x)sin(y)</t>
   </si>
   <si>
-    <t>--------------------------------------------------------------------------------------------- Refresher ends here-----------------------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>Continuity Example</t>
-  </si>
-  <si>
-    <t>f(0) is discontinous at x =0</t>
-  </si>
-  <si>
-    <t>it is called discontinpos function at x=0</t>
-  </si>
-  <si>
-    <t>A function os said to be continous at c when limit as x--&gt;c (from both sides) approaches the value of function at f(c)</t>
-  </si>
-  <si>
-    <t>To find if a function is continous, see if the functions is defined for all input values . In eaxmple above f is defined for &lt;2 , =2  and &gt;2 , so it is defined for all</t>
-  </si>
-  <si>
-    <t>A real function f is said to be continous if it is continous on every point in domain of f</t>
+    <t>d/dx of various trignometric functions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,346 +136,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -507,307 +153,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -818,7 +175,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -840,7 +197,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -882,7 +239,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -924,7 +281,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -966,7 +323,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1008,7 +365,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1050,7 +407,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1092,7 +449,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1134,7 +491,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1176,7 +533,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1218,7 +575,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1260,7 +617,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1302,7 +659,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1344,7 +701,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1386,7 +743,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1428,7 +785,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1470,7 +827,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1512,7 +869,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1554,7 +911,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1596,7 +953,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1619,168 +976,40 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>54610</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId20"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2171700" y="28365450"/>
-          <a:ext cx="1885950" cy="835660"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId21"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3971925" y="29813250"/>
-          <a:ext cx="2819400" cy="638175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>494030</xdr:colOff>
-      <xdr:row>161</xdr:row>
-      <xdr:rowOff>142240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>178</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId22"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4094480" y="30812740"/>
-          <a:ext cx="5506720" cy="3181985"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>188</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>443230</xdr:colOff>
-      <xdr:row>196</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId23"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3438525" y="35848290"/>
-          <a:ext cx="1805305" cy="1546860"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>223235</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9344025" y="20897849"/>
+          <a:ext cx="2880710" cy="2847975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2040,21 +1269,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:Q189"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="M192" sqref="M192"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2062,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2070,27 +1299,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:3">
+    <row r="4" spans="1:4">
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:3">
+    <row r="5" spans="1:4">
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
+    <row r="6" spans="1:4">
       <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="4:4">
+    <row r="10" spans="1:4">
       <c r="D10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="4:4">
+    <row r="12" spans="1:4">
       <c r="D12" t="s">
         <v>8</v>
       </c>
@@ -2100,52 +1329,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="5:5">
+    <row r="33" spans="4:5">
       <c r="E33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:5">
       <c r="D37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="5:5">
+    <row r="38" spans="4:5">
       <c r="E38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="5:5">
+    <row r="39" spans="4:5">
       <c r="E39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="5:5">
+    <row r="40" spans="4:5">
       <c r="E40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="5:5">
+    <row r="41" spans="4:5">
       <c r="E41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="3:3">
+    <row r="52" spans="3:17">
       <c r="C52" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="6:6">
+    <row r="55" spans="3:17">
       <c r="F55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="13:13">
+    <row r="56" spans="3:17">
       <c r="M56">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="13:17">
+    <row r="58" spans="3:17">
       <c r="M58">
         <v>2</v>
       </c>
@@ -2156,7 +1385,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="13:17">
+    <row r="59" spans="3:17">
       <c r="M59">
         <v>3</v>
       </c>
@@ -2167,7 +1396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="13:15">
+    <row r="60" spans="3:17">
       <c r="M60">
         <v>4</v>
       </c>
@@ -2175,7 +1404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="13:15">
+    <row r="61" spans="3:17">
       <c r="M61">
         <v>5</v>
       </c>
@@ -2183,7 +1412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="13:15">
+    <row r="62" spans="3:17">
       <c r="M62">
         <v>6</v>
       </c>
@@ -2191,7 +1420,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="13:15">
+    <row r="63" spans="3:17">
       <c r="M63">
         <v>7</v>
       </c>
@@ -2199,7 +1428,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="13:15">
+    <row r="64" spans="3:17">
       <c r="M64">
         <v>8</v>
       </c>
@@ -2207,7 +1436,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="13:15">
+    <row r="65" spans="4:15">
       <c r="M65">
         <v>9</v>
       </c>
@@ -2215,22 +1444,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="13:13">
+    <row r="66" spans="4:15">
       <c r="M66">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="13:13">
+    <row r="67" spans="4:15">
       <c r="M67">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="13:13">
+    <row r="68" spans="4:15">
       <c r="M68">
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="13:15">
+    <row r="70" spans="4:15">
       <c r="M70">
         <v>13</v>
       </c>
@@ -2238,7 +1467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="13:15">
+    <row r="71" spans="4:15">
       <c r="M71">
         <v>14</v>
       </c>
@@ -2246,7 +1475,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="4:13">
+    <row r="72" spans="4:15">
       <c r="D72">
         <v>23</v>
       </c>
@@ -2254,27 +1483,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="13:13">
+    <row r="74" spans="4:15">
       <c r="M74">
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="13:13">
+    <row r="77" spans="4:15">
       <c r="M77">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="13:13">
+    <row r="80" spans="4:15">
       <c r="M80">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="13:13">
+    <row r="82" spans="4:13">
       <c r="M82">
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="4:5">
+    <row r="83" spans="4:13">
       <c r="D83">
         <v>24</v>
       </c>
@@ -2293,7 +1522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="4:5">
+    <row r="85" spans="4:13">
       <c r="D85">
         <v>26</v>
       </c>
@@ -2312,7 +1541,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="4:5">
+    <row r="87" spans="4:13">
       <c r="D87">
         <v>28</v>
       </c>
@@ -2320,84 +1549,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="13:13">
+    <row r="88" spans="4:13">
       <c r="M88">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="12:12">
+    <row r="94" spans="4:13">
       <c r="L94">
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="12:12">
+    <row r="98" spans="12:17">
       <c r="L98">
         <v>30</v>
       </c>
     </row>
+    <row r="108" spans="12:17">
+      <c r="Q108" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148">
-        <v>1</v>
-      </c>
-      <c r="B148" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="149" spans="4:9">
-      <c r="D149">
-        <v>1</v>
-      </c>
-      <c r="I149" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="150" spans="9:9">
-      <c r="I150" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="156" spans="4:6">
-      <c r="D156">
-        <v>2</v>
-      </c>
-      <c r="F156" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="162" spans="4:4">
-      <c r="D162">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="183" spans="4:6">
-      <c r="D183">
-        <v>4</v>
-      </c>
-      <c r="F183" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="186" spans="4:6">
-      <c r="D186">
-        <v>5</v>
-      </c>
-      <c r="F186" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="189" spans="4:4">
-      <c r="D189">
-        <v>6</v>
-      </c>
+      <c r="A145" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
continuity and diffrenciability updated
</commit_message>
<xml_diff>
--- a/12/12ContinuityAndDiffrentiability.xlsx
+++ b/12/12ContinuityAndDiffrentiability.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19635" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19635" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t xml:space="preserve">1) </t>
   </si>
@@ -122,6 +124,90 @@
   </si>
   <si>
     <t>d/dx of various trignometric functions</t>
+  </si>
+  <si>
+    <t>Calculus is a branch that studies change in the function with change in its domain value and uses LIMITs</t>
+  </si>
+  <si>
+    <t>Limit is used when we want to find the value of a function in NEIGHBOURHOOD of a Point in DOMAIN of the function</t>
+  </si>
+  <si>
+    <t>f(x) = x+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> here f = 6 at x=3, but in limit we find the value of fucntion in neighbouhood of 3(2.9999 or 3.0001) what is the value ?? Limit tells us that</t>
+  </si>
+  <si>
+    <t>x can approach 3 from left and right side,</t>
+  </si>
+  <si>
+    <t>When A function has a value at a point AND  right hand limit and left hand limit appoach to same point, then we say LIMIT EXISTS at that point of function</t>
+  </si>
+  <si>
+    <t>Value of function at a point is a different thing and LIMIT value in the neighbourhood of this point is a different thing. That’s why we try not to get 0 in denominator of the function</t>
+  </si>
+  <si>
+    <t>Derivative:</t>
+  </si>
+  <si>
+    <t>How a function changes with change in the value of its domain</t>
+  </si>
+  <si>
+    <t>d/dx</t>
+  </si>
+  <si>
+    <t>12 Starts -----------------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Continuity : Why continuity ?</t>
+  </si>
+  <si>
+    <t>Because, the derivative of a function exits at a point, ONLY if the function is continous at that point</t>
+  </si>
+  <si>
+    <t>If function is discontinous at p (i.e. there is a break at p) then limit will not exist</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is velocity ? </t>
+  </si>
+  <si>
+    <t>Change in distace with time</t>
+  </si>
+  <si>
+    <t>Average Velocity</t>
+  </si>
+  <si>
+    <t>Instantanious Velocity</t>
+  </si>
+  <si>
+    <t>: here delta t --&gt; 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A tangent is drawn at point P and the slope (tan theta) of this tangent is called derivative of the function at point P </t>
+  </si>
+  <si>
+    <t>Discontinous Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a finction is discontinous at some point, then we can </t>
+  </si>
+  <si>
+    <t>not draw any tangent at that point, so its slope</t>
+  </si>
+  <si>
+    <t>can not be found AT that point (on other points we can)</t>
+  </si>
+  <si>
+    <t>So Discontinuity is AT A POINT (not all across the function)</t>
+  </si>
+  <si>
+    <t>Definition of continuity</t>
+  </si>
+  <si>
+    <t>A function is said to be continous if it is continous at every point in domain of f</t>
   </si>
 </sst>
 </file>
@@ -180,13 +266,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -222,13 +308,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>210185</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -264,13 +350,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>122555</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>84455</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -306,13 +392,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -348,13 +434,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -390,13 +476,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -432,13 +518,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>266065</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -474,13 +560,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -516,13 +602,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -558,13 +644,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -600,13 +686,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -642,13 +728,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -684,13 +770,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -726,13 +812,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -768,13 +854,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -810,13 +896,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -852,13 +938,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>156</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -894,13 +980,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -936,13 +1022,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -978,13 +1064,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>223235</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>143</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1005,6 +1091,656 @@
         <a:xfrm>
           <a:off x="9344025" y="20897849"/>
           <a:ext cx="2880710" cy="2847975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>169015</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10572750" y="685800"/>
+          <a:ext cx="923925" cy="435715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>177188</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7524751" y="1981201"/>
+          <a:ext cx="4053862" cy="1790699"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>141308</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1030" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9515476" y="30184725"/>
+          <a:ext cx="1847849" cy="1960583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>573051</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1032" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3028951" y="32689800"/>
+          <a:ext cx="4745000" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>124836</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1034" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5648325" y="35118676"/>
+          <a:ext cx="1790700" cy="1010660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>261893</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1036" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7820025" y="37338000"/>
+          <a:ext cx="3243218" cy="2228850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>74904</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1038" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4724400" y="39814500"/>
+          <a:ext cx="2352675" cy="1408404"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2826</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4381500" cy="2860326"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>80964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2055" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5943600" y="28576"/>
+          <a:ext cx="5438775" cy="2719388"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>143854</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2057" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4048125"/>
+          <a:ext cx="6781800" cy="3715729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>174917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2059" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8191501"/>
+          <a:ext cx="6686550" cy="3794416"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>135086</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2061" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19051" y="12172950"/>
+          <a:ext cx="6315074" cy="3583136"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>11956</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3074" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5295900" cy="2678956"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>140328</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3076" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6400800" y="0"/>
+          <a:ext cx="5321928" cy="2676524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3078" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3019425"/>
+          <a:ext cx="3905250" cy="3200400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3080" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="123825" y="6591300"/>
+          <a:ext cx="7886700" cy="4476750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1275,15 +2011,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q145"/>
+  <dimension ref="A1:Q209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="F203" sqref="F203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1291,286 +2027,445 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="B3" t="s">
+    <row r="4" spans="1:5">
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="C4" t="s">
+    <row r="23" spans="2:4">
+      <c r="C23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="C5" t="s">
+    <row r="24" spans="2:4">
+      <c r="C24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="C6" t="s">
+    <row r="25" spans="2:4">
+      <c r="C25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="D10" t="s">
+    <row r="29" spans="2:4">
+      <c r="D29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="D12" t="s">
+    <row r="31" spans="2:4">
+      <c r="D31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="4:4">
-      <c r="D32" t="s">
+    <row r="51" spans="4:5">
+      <c r="D51" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="4:5">
-      <c r="E33" t="s">
+    <row r="52" spans="4:5">
+      <c r="E52" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="4:5">
-      <c r="D37" t="s">
+    <row r="56" spans="4:5">
+      <c r="D56" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="4:5">
-      <c r="E38" t="s">
+    <row r="57" spans="4:5">
+      <c r="E57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="4:5">
-      <c r="E39" t="s">
+    <row r="58" spans="4:5">
+      <c r="E58" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="4:5">
-      <c r="E40" t="s">
+    <row r="59" spans="4:5">
+      <c r="E59" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="4:5">
-      <c r="E41" t="s">
+    <row r="60" spans="4:5">
+      <c r="E60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="3:17">
-      <c r="C52" t="s">
+    <row r="71" spans="3:17">
+      <c r="C71" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="3:17">
-      <c r="F55" t="s">
+    <row r="74" spans="3:17">
+      <c r="F74" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="3:17">
-      <c r="M56">
+    <row r="75" spans="3:17">
+      <c r="M75">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="3:17">
-      <c r="M58">
+    <row r="77" spans="3:17">
+      <c r="M77">
         <v>2</v>
       </c>
-      <c r="O58" t="s">
+      <c r="O77" t="s">
         <v>18</v>
       </c>
-      <c r="Q58" t="s">
+      <c r="Q77" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="3:17">
-      <c r="M59">
+    <row r="78" spans="3:17">
+      <c r="M78">
         <v>3</v>
       </c>
-      <c r="O59" t="s">
+      <c r="O78" t="s">
         <v>20</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="Q78" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="3:17">
-      <c r="M60">
+    <row r="79" spans="3:17">
+      <c r="M79">
         <v>4</v>
       </c>
-      <c r="O60" t="s">
+      <c r="O79" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="3:17">
-      <c r="M61">
+    <row r="80" spans="3:17">
+      <c r="M80">
         <v>5</v>
       </c>
-      <c r="O61" t="s">
+      <c r="O80" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="3:17">
-      <c r="M62">
+    <row r="81" spans="4:15">
+      <c r="M81">
         <v>6</v>
       </c>
-      <c r="O62" t="s">
+      <c r="O81" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="3:17">
-      <c r="M63">
+    <row r="82" spans="4:15">
+      <c r="M82">
         <v>7</v>
       </c>
-      <c r="O63" t="s">
+      <c r="O82" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="3:17">
-      <c r="M64">
+    <row r="83" spans="4:15">
+      <c r="M83">
         <v>8</v>
       </c>
-      <c r="O64" t="s">
+      <c r="O83" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="4:15">
-      <c r="M65">
+    <row r="84" spans="4:15">
+      <c r="M84">
         <v>9</v>
       </c>
-      <c r="O65" t="s">
+      <c r="O84" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="4:15">
-      <c r="M66">
+    <row r="85" spans="4:15">
+      <c r="M85">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="4:15">
-      <c r="M67">
+    <row r="86" spans="4:15">
+      <c r="M86">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="4:15">
-      <c r="M68">
+    <row r="87" spans="4:15">
+      <c r="M87">
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="4:15">
-      <c r="M70">
+    <row r="89" spans="4:15">
+      <c r="M89">
         <v>13</v>
       </c>
-      <c r="O70" t="s">
+      <c r="O89" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="4:15">
-      <c r="M71">
+    <row r="90" spans="4:15">
+      <c r="M90">
         <v>14</v>
       </c>
-      <c r="O71" t="s">
+      <c r="O90" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="4:15">
-      <c r="D72">
+    <row r="91" spans="4:15">
+      <c r="D91">
         <v>23</v>
       </c>
-      <c r="M72">
+      <c r="M91">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="4:15">
-      <c r="M74">
+    <row r="93" spans="4:15">
+      <c r="M93">
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="4:15">
-      <c r="M77">
+    <row r="96" spans="4:15">
+      <c r="M96">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="4:15">
-      <c r="M80">
+    <row r="99" spans="4:13">
+      <c r="M99">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="4:13">
-      <c r="M82">
+    <row r="101" spans="4:13">
+      <c r="M101">
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="4:13">
-      <c r="D83">
+    <row r="102" spans="4:13">
+      <c r="D102">
         <v>24</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E102" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="4:13">
-      <c r="D84">
+    <row r="103" spans="4:13">
+      <c r="D103">
         <v>25</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E103" t="s">
         <v>31</v>
       </c>
-      <c r="M84">
+      <c r="M103">
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="4:13">
-      <c r="D85">
+    <row r="104" spans="4:13">
+      <c r="D104">
         <v>26</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E104" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="4:13">
-      <c r="D86">
+    <row r="105" spans="4:13">
+      <c r="D105">
         <v>27</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E105" t="s">
         <v>33</v>
       </c>
-      <c r="M86">
+      <c r="M105">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="4:13">
-      <c r="D87">
+    <row r="106" spans="4:13">
+      <c r="D106">
         <v>28</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E106" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="4:13">
-      <c r="M88">
+    <row r="107" spans="4:13">
+      <c r="M107">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="4:13">
-      <c r="L94">
+    <row r="113" spans="3:17">
+      <c r="L113">
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="12:17">
-      <c r="L98">
+    <row r="117" spans="3:17">
+      <c r="L117">
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="12:17">
-      <c r="Q108" t="s">
+    <row r="122" spans="3:17">
+      <c r="C122" t="s">
+        <v>43</v>
+      </c>
+      <c r="E122" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="123" spans="3:17">
+      <c r="E123" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="127" spans="3:17">
+      <c r="Q127" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
-      <c r="A145" s="1"/>
+    <row r="162" spans="1:6">
+      <c r="A162" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="1"/>
+      <c r="B164" t="s">
+        <v>47</v>
+      </c>
+      <c r="F164" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="F166" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="B170" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="C171" t="s">
+        <v>51</v>
+      </c>
+      <c r="F171" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="D174" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="185" spans="4:7">
+      <c r="D185" t="s">
+        <v>54</v>
+      </c>
+      <c r="G185" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="193" spans="4:7">
+      <c r="G193" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="196" spans="4:7">
+      <c r="D196" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="198" spans="4:7">
+      <c r="F198" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="199" spans="4:7">
+      <c r="G199" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="200" spans="4:7">
+      <c r="G200" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="201" spans="4:7">
+      <c r="G201" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="209" spans="5:5">
+      <c r="E209" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>